<commit_message>
Capitalization of Pop item bank
</commit_message>
<xml_diff>
--- a/data_raw/item_banks/pop_item_bank.xlsx
+++ b/data_raw/item_banks/pop_item_bank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpiquiz\data_raw\item_banks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA13BE28-B174-4E6A-B6F1-67424A25C45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C766DD05-7079-47C4-95CA-D4CA969D2758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E24A31F9-3C3D-E74D-9343-50AC9B0E25D1}"/>
   </bookViews>
@@ -27,246 +27,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="85">
   <si>
-    <t>taylor swift</t>
-  </si>
-  <si>
-    <t>robbie williams</t>
-  </si>
-  <si>
-    <t>nelly fortado</t>
-  </si>
-  <si>
-    <t>kesha</t>
-  </si>
-  <si>
-    <t>usher</t>
-  </si>
-  <si>
-    <t>olivia rodrigo</t>
-  </si>
-  <si>
-    <t>the weeknd</t>
-  </si>
-  <si>
-    <t>taio cruz</t>
-  </si>
-  <si>
-    <t>katy perry</t>
-  </si>
-  <si>
-    <t>fergie</t>
-  </si>
-  <si>
     <t>will.i.am</t>
   </si>
   <si>
-    <t>akon</t>
-  </si>
-  <si>
-    <t>bruno mars</t>
-  </si>
-  <si>
-    <t>ed sheeran</t>
-  </si>
-  <si>
-    <t>justin bieber</t>
-  </si>
-  <si>
-    <t>michael bublé</t>
-  </si>
-  <si>
-    <t>harry styles</t>
-  </si>
-  <si>
-    <t>sam smith</t>
-  </si>
-  <si>
-    <t>shawn mendes</t>
-  </si>
-  <si>
-    <t>christina aguilera</t>
-  </si>
-  <si>
-    <t>adele</t>
-  </si>
-  <si>
-    <t>dua lipa</t>
-  </si>
-  <si>
-    <t>lady gaga</t>
-  </si>
-  <si>
-    <t>anastacia</t>
-  </si>
-  <si>
-    <t>billie eilish</t>
-  </si>
-  <si>
-    <t>miley cyrus</t>
-  </si>
-  <si>
-    <t>britney spears</t>
-  </si>
-  <si>
-    <t>mariah carey</t>
-  </si>
-  <si>
-    <t>lana del rey</t>
-  </si>
-  <si>
-    <t>eminem</t>
-  </si>
-  <si>
-    <t>nina simone</t>
-  </si>
-  <si>
-    <t>sarah vaughan</t>
-  </si>
-  <si>
-    <t>kurt cobain</t>
-  </si>
-  <si>
-    <t>billy joe armstrong</t>
-  </si>
-  <si>
-    <t>ray charles</t>
-  </si>
-  <si>
-    <t>jim morrison</t>
-  </si>
-  <si>
-    <t>roger cicero</t>
-  </si>
-  <si>
-    <t>50 cent</t>
-  </si>
-  <si>
-    <t>charli xcx</t>
-  </si>
-  <si>
-    <t>caroline polachek</t>
-  </si>
-  <si>
-    <t>chris martin</t>
-  </si>
-  <si>
-    <t>adam levine</t>
-  </si>
-  <si>
-    <t>miguel</t>
-  </si>
-  <si>
-    <t>alee</t>
-  </si>
-  <si>
-    <t>liz anderson</t>
-  </si>
-  <si>
-    <t>ashley arrison</t>
-  </si>
-  <si>
-    <t>keith bryant</t>
-  </si>
-  <si>
-    <t>chris cagle</t>
-  </si>
-  <si>
-    <t>deana carter</t>
-  </si>
-  <si>
-    <t>diane chase</t>
-  </si>
-  <si>
-    <t>amy dalley</t>
-  </si>
-  <si>
-    <t>roxie dean</t>
-  </si>
-  <si>
-    <t>travis denning</t>
-  </si>
-  <si>
-    <t>josh gracin</t>
-  </si>
-  <si>
-    <t>eva O</t>
-  </si>
-  <si>
-    <t>courtney love</t>
-  </si>
-  <si>
-    <t>sierra kay</t>
-  </si>
-  <si>
-    <t>charlie puth</t>
-  </si>
-  <si>
-    <t>masta ace</t>
-  </si>
-  <si>
-    <t>benzino</t>
-  </si>
-  <si>
-    <t>david archuleta</t>
-  </si>
-  <si>
-    <t>emilio</t>
-  </si>
-  <si>
-    <t>geza X</t>
-  </si>
-  <si>
-    <t>krizz kaliko</t>
-  </si>
-  <si>
-    <t>alecia elliott</t>
-  </si>
-  <si>
-    <t>cassidy</t>
-  </si>
-  <si>
-    <t>don toliver</t>
-  </si>
-  <si>
-    <t>slowthai</t>
-  </si>
-  <si>
-    <t>amil</t>
-  </si>
-  <si>
-    <t>tiffany foxx</t>
-  </si>
-  <si>
-    <t>mia X</t>
-  </si>
-  <si>
-    <t>nonchalant</t>
-  </si>
-  <si>
-    <t>khia</t>
-  </si>
-  <si>
-    <t>kaliii</t>
-  </si>
-  <si>
-    <t>luciano</t>
-  </si>
-  <si>
-    <t>santos</t>
-  </si>
-  <si>
-    <t>ludacris</t>
-  </si>
-  <si>
-    <t>billie holiday</t>
-  </si>
-  <si>
-    <t>ayliva</t>
-  </si>
-  <si>
-    <t>kim petras</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -280,6 +43,243 @@
   </si>
   <si>
     <t>item_id</t>
+  </si>
+  <si>
+    <t>Shawn Mendes</t>
+  </si>
+  <si>
+    <t>Chris Martin</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Adam Levine</t>
+  </si>
+  <si>
+    <t>Robbie Williams</t>
+  </si>
+  <si>
+    <t>Usher</t>
+  </si>
+  <si>
+    <t>The Weeknd</t>
+  </si>
+  <si>
+    <t>Taio Cruz</t>
+  </si>
+  <si>
+    <t>Akon</t>
+  </si>
+  <si>
+    <t>Bruno Mars</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Ed Sheeran</t>
+  </si>
+  <si>
+    <t>Emilio</t>
+  </si>
+  <si>
+    <t>Justin Bieber</t>
+  </si>
+  <si>
+    <t>Michael Bublé</t>
+  </si>
+  <si>
+    <t>Harry Styles</t>
+  </si>
+  <si>
+    <t>Sam Smith</t>
+  </si>
+  <si>
+    <t>David Archuleta</t>
+  </si>
+  <si>
+    <t>Charlie Puth</t>
+  </si>
+  <si>
+    <t>Taylor Swift</t>
+  </si>
+  <si>
+    <t>Lana del Rey</t>
+  </si>
+  <si>
+    <t>Nelly Fortado</t>
+  </si>
+  <si>
+    <t>Ayliva</t>
+  </si>
+  <si>
+    <t>Kesha</t>
+  </si>
+  <si>
+    <t>Charli XCX</t>
+  </si>
+  <si>
+    <t>Olivia Rodrigo</t>
+  </si>
+  <si>
+    <t>Katy Perry</t>
+  </si>
+  <si>
+    <t>Fergie</t>
+  </si>
+  <si>
+    <t>Caroline Polachek</t>
+  </si>
+  <si>
+    <t>Christina Aguilera</t>
+  </si>
+  <si>
+    <t>Adele</t>
+  </si>
+  <si>
+    <t>Dua Lipa</t>
+  </si>
+  <si>
+    <t>Lady Gaga</t>
+  </si>
+  <si>
+    <t>Mariah Carey</t>
+  </si>
+  <si>
+    <t>Anastacia</t>
+  </si>
+  <si>
+    <t>Kim Petras</t>
+  </si>
+  <si>
+    <t>Billie Eilish</t>
+  </si>
+  <si>
+    <t>Miley Cyrus</t>
+  </si>
+  <si>
+    <t>Britney Spears</t>
+  </si>
+  <si>
+    <t>Eminem</t>
+  </si>
+  <si>
+    <t>Kurt Cobain</t>
+  </si>
+  <si>
+    <t>Billy Joe Armstrong</t>
+  </si>
+  <si>
+    <t>Ray Charles</t>
+  </si>
+  <si>
+    <t>Jim Morrison</t>
+  </si>
+  <si>
+    <t>Roger Cicero</t>
+  </si>
+  <si>
+    <t>50 Cent</t>
+  </si>
+  <si>
+    <t>Keith Bryant</t>
+  </si>
+  <si>
+    <t>Chris Cagle</t>
+  </si>
+  <si>
+    <t>Luciano</t>
+  </si>
+  <si>
+    <t>Josh Gracin</t>
+  </si>
+  <si>
+    <t>Ludacris</t>
+  </si>
+  <si>
+    <t>Travis Denning</t>
+  </si>
+  <si>
+    <t>Geza X</t>
+  </si>
+  <si>
+    <t>Krizz Kaliko</t>
+  </si>
+  <si>
+    <t>Benzino</t>
+  </si>
+  <si>
+    <t>Masta Ace</t>
+  </si>
+  <si>
+    <t>Cassidy</t>
+  </si>
+  <si>
+    <t>Don Toliver</t>
+  </si>
+  <si>
+    <t>Slowthai</t>
+  </si>
+  <si>
+    <t>Nina Simone</t>
+  </si>
+  <si>
+    <t>Sarah Vaughan</t>
+  </si>
+  <si>
+    <t>Diane Chase</t>
+  </si>
+  <si>
+    <t>Alee</t>
+  </si>
+  <si>
+    <t>Liz Anderson</t>
+  </si>
+  <si>
+    <t>Ashley Arrison</t>
+  </si>
+  <si>
+    <t>Deana Carter</t>
+  </si>
+  <si>
+    <t>Billie Holiday</t>
+  </si>
+  <si>
+    <t>Amy Dalley</t>
+  </si>
+  <si>
+    <t>Roxie Dean</t>
+  </si>
+  <si>
+    <t>Eva O</t>
+  </si>
+  <si>
+    <t>Alecia Elliott</t>
+  </si>
+  <si>
+    <t>Courtney Love</t>
+  </si>
+  <si>
+    <t>Sierra Kay</t>
+  </si>
+  <si>
+    <t>Amil</t>
+  </si>
+  <si>
+    <t>Tiffany Foxx</t>
+  </si>
+  <si>
+    <t>Mia X</t>
+  </si>
+  <si>
+    <t>Nonchalant</t>
+  </si>
+  <si>
+    <t>Khia</t>
+  </si>
+  <si>
+    <t>Kaliii</t>
   </si>
 </sst>
 </file>
@@ -662,7 +662,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A84A43B-F196-9D46-B81A-58E8FA543359}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="111" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -674,13 +676,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -688,10 +690,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -700,10 +702,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2"/>
       <c r="F3" s="1"/>
@@ -715,10 +717,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -727,10 +729,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -739,10 +741,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -751,10 +753,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -763,10 +765,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -775,10 +777,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -787,10 +789,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -799,10 +801,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -811,10 +813,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -823,10 +825,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -835,10 +837,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -847,10 +849,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -859,10 +861,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -871,10 +873,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -883,10 +885,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -895,10 +897,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -907,10 +909,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -919,10 +921,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -931,10 +933,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -943,10 +945,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -955,10 +957,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,10 +969,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -979,10 +981,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,10 +993,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1003,10 +1005,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1015,10 +1017,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1027,10 +1029,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1039,10 +1041,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1051,10 +1053,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1063,10 +1065,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1075,10 +1077,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1087,10 +1089,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,10 +1101,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1111,10 +1113,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1123,10 +1125,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1135,10 +1137,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1147,10 +1149,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,10 +1161,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1171,10 +1173,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1183,10 +1185,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1195,10 +1197,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1207,10 +1209,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1219,10 +1221,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1231,10 +1233,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1243,10 +1245,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1255,10 +1257,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1267,10 +1269,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1279,10 +1281,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1291,10 +1293,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1303,10 +1305,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1315,10 +1317,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1327,10 +1329,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1339,10 +1341,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1351,10 +1353,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1363,10 +1365,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1375,10 +1377,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1387,10 +1389,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1399,10 +1401,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1411,10 +1413,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1423,10 +1425,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1435,10 +1437,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C64" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1447,10 +1449,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1459,10 +1461,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1471,10 +1473,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1483,10 +1485,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1495,10 +1497,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1507,10 +1509,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1519,10 +1521,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C71" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1531,10 +1533,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="C72" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1543,10 +1545,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C73" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1555,10 +1557,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="C74" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1567,10 +1569,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="C75" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1579,10 +1581,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C76" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1591,10 +1593,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C77" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1603,10 +1605,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C78" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1615,10 +1617,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C79" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1627,10 +1629,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1639,10 +1641,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C81" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>